<commit_message>
fix xlsx column names
</commit_message>
<xml_diff>
--- a/R_Beech_Roots.xlsx
+++ b/R_Beech_Roots.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Research_Beech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543E5D7E-9876-4ADE-8D65-64BAEB1E7EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976D8EAA-B9CE-421F-B9B1-7637213EEA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="280">
   <si>
     <t>id</t>
   </si>
@@ -436,31 +436,31 @@
   </si>
   <si>
     <t>●個体番号A柄山樹高15cm未満、B柄山樹高15cm以上30cm未満、C柄山樹高30cm以上、O大洞、H聖山</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>site</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>KRY</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>OBR</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>HJY</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>Log</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>Remarks</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>主幹折れ</t>
@@ -470,73 +470,73 @@
     <rPh sb="2" eb="3">
       <t xml:space="preserve">オレ </t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>trunk_length</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>trunk_tilt</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>ground_origin_ratio</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>slope</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>D0</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>height</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>length</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>total_length</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>L/H</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>D_origine</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>age</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>頓所</t>
     <rPh sb="0" eb="2">
       <t>トンドコロ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>聖山</t>
     <rPh sb="0" eb="2">
       <t>ヒジリヤマ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>NA</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>c</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N17E</t>
@@ -549,7 +549,7 @@
     <rPh sb="1" eb="2">
       <t>オ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N32E</t>
@@ -565,11 +565,11 @@
     <rPh sb="0" eb="2">
       <t>オオボラ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>b</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N12E</t>
@@ -582,7 +582,7 @@
     <rPh sb="5" eb="6">
       <t>オ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N28E</t>
@@ -607,14 +607,14 @@
     <rPh sb="6" eb="8">
       <t>サカイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>柄山</t>
     <rPh sb="0" eb="2">
       <t>カラヤマ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>S22E</t>
@@ -630,7 +630,7 @@
     <rPh sb="6" eb="8">
       <t>イダ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>依田、大越</t>
@@ -640,11 +640,11 @@
     <rPh sb="3" eb="5">
       <t>オオゴシ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>a</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>主幹折れ</t>
@@ -654,7 +654,7 @@
     <rPh sb="2" eb="3">
       <t>オ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>調査日</t>
@@ -664,28 +664,28 @@
     <rPh sb="2" eb="3">
       <t>ビ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>調査者</t>
     <rPh sb="0" eb="3">
       <t>チョウサシャ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>調査地</t>
     <rPh sb="0" eb="3">
       <t>チョウサチ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>備考</t>
     <rPh sb="0" eb="2">
       <t>ビコウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>埋幹部年齢</t>
@@ -698,7 +698,7 @@
     <rPh sb="3" eb="5">
       <t>ネンレイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>発育原点年輪数
@@ -715,7 +715,7 @@
     <rPh sb="6" eb="7">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>発育原点直径平均
@@ -732,7 +732,7 @@
     <rPh sb="6" eb="8">
       <t>ヘイキン</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>発育原点直径②
@@ -746,7 +746,7 @@
     <rPh sb="4" eb="6">
       <t>チョッケイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>発育原点直径①
@@ -760,7 +760,7 @@
     <rPh sb="4" eb="6">
       <t>チョッケイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>地際年輪数</t>
@@ -776,7 +776,7 @@
     <rPh sb="4" eb="5">
       <t>スウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>芽鱗根数
@@ -790,7 +790,7 @@
     <rPh sb="6" eb="7">
       <t>コ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>樹幹傾斜度
@@ -804,7 +804,7 @@
     <rPh sb="4" eb="5">
       <t>ド</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>埋幹部重量
@@ -821,7 +821,7 @@
     <rPh sb="6" eb="8">
       <t>ワリアイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥後埋幹部
@@ -841,7 +841,7 @@
     <rPh sb="7" eb="9">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥後発育原点下
@@ -852,7 +852,7 @@
     <rPh sb="2" eb="3">
       <t>ゴ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥前発育原点下
@@ -881,43 +881,43 @@
     <rPh sb="11" eb="13">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>22.5～25.0</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>20.0～22.5</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>17.5～20.0</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>15.0～17.5</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>12.5～15.0</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>10.0～12.5</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>7.5～10.0</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>5.0～7.5</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>2.5～5.0</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥前発育原点下
@@ -943,14 +943,14 @@
     <rPh sb="10" eb="12">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>T/R比</t>
     <rPh sb="3" eb="4">
       <t>ヒ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥後稚樹全重量[g]</t>
@@ -969,7 +969,7 @@
     <rPh sb="7" eb="9">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥後地下部総重量[g]</t>
@@ -988,7 +988,7 @@
     <rPh sb="7" eb="10">
       <t>ソウジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥後地下部重量0〜2.5cm[g]</t>
@@ -1007,7 +1007,7 @@
     <rPh sb="7" eb="9">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥後地上部重量[g]</t>
@@ -1023,7 +1023,7 @@
     <rPh sb="7" eb="9">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥前稚樹全重量[g]</t>
@@ -1042,7 +1042,7 @@
     <rPh sb="7" eb="9">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥前地下部総重量[g]</t>
@@ -1061,7 +1061,7 @@
     <rPh sb="7" eb="10">
       <t>ソウジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥前地下部重量0～2.5 cm[g]</t>
@@ -1080,7 +1080,7 @@
     <rPh sb="7" eb="9">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>乾燥前地上部
@@ -1097,7 +1097,7 @@
     <rPh sb="7" eb="9">
       <t>ジュウリョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>水平長さ
@@ -1108,7 +1108,7 @@
     <rPh sb="2" eb="3">
       <t>ナガ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>垂直長さ
@@ -1119,14 +1119,14 @@
     <rPh sb="2" eb="3">
       <t>ナガ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>L/H比</t>
     <rPh sb="3" eb="4">
       <t>ヒ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>樹幹長
@@ -1137,7 +1137,7 @@
     <rPh sb="2" eb="3">
       <t>チョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>全長
@@ -1145,7 +1145,7 @@
     <rPh sb="0" eb="2">
       <t>ゼンチョウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>階層区分</t>
@@ -1155,7 +1155,7 @@
     <rPh sb="2" eb="4">
       <t>クブン</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>樹高
@@ -1163,7 +1163,7 @@
     <rPh sb="0" eb="2">
       <t>ジュコウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>地際直径平均
@@ -1180,7 +1180,7 @@
     <rPh sb="4" eb="6">
       <t>ヘイキン</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>地際直径２
@@ -1194,7 +1194,7 @@
     <rPh sb="2" eb="4">
       <t>チョッケイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>地際直径１
@@ -1208,7 +1208,7 @@
     <rPh sb="2" eb="4">
       <t>チョッケイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>斜面傾斜
@@ -1219,7 +1219,7 @@
     <rPh sb="2" eb="4">
       <t>ケイシャ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>斜面方位</t>
@@ -1229,7 +1229,7 @@
     <rPh sb="2" eb="4">
       <t>ホウイ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>個体ID</t>
@@ -1239,62 +1239,62 @@
     <rPh sb="2" eb="4">
       <t>バンゴウ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>●個体番号A柄山樹高15cm未満、B柄山樹高15cm以上30cm未満、C柄山樹高30cm以上、O大洞、H聖山</t>
   </si>
   <si>
     <t>N17E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N32E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N50E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N73E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>H2</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>H1</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N12E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N28E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N27E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N38E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>O2</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>N63E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>O1</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>柄山地区</t>
@@ -1304,18 +1304,18 @@
     <rPh sb="2" eb="4">
       <t>チク</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
     <t>C2</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>C1</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>柳澤、保坂</t>
@@ -1325,94 +1325,78 @@
     <rPh sb="3" eb="5">
       <t>ホサカ</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>B2</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>B1</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>S22E</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>A1</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>採取有無</t>
     <rPh sb="0" eb="2">
       <t>サイシュウム</t>
     </rPh>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>id</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>slope</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>D0</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>Height</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>total_length</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>Length</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>L/H</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>T/R</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>trunk_weight</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>trunk_inclination</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>D0_age</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>D_origine</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>D_origine_age</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="9"/>
   </si>
   <si>
     <t>HJR</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>root width</t>
-    <phoneticPr fontId="8"/>
-  </si>
-  <si>
-    <t>root depth</t>
-    <phoneticPr fontId="8"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>R用データ抽出</t>
@@ -1422,7 +1406,7 @@
     <rPh sb="5" eb="7">
       <t xml:space="preserve">チュウシュツ </t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <t>buried_trunk_weight</t>
@@ -1477,6 +1461,21 @@
   </si>
   <si>
     <t>D_origine_age</t>
+  </si>
+  <si>
+    <t>L.H</t>
+  </si>
+  <si>
+    <t>T.R</t>
+  </si>
+  <si>
+    <t>buried_trunk_.</t>
+  </si>
+  <si>
+    <t>root.width</t>
+  </si>
+  <si>
+    <t>root.depth</t>
   </si>
 </sst>
 </file>
@@ -1486,11 +1485,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1607,83 +1613,83 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6215,7 +6221,7 @@
     <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:J116" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="7"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait"/>
@@ -8595,7 +8601,7 @@
     <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:P26" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="7"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape"/>
@@ -13415,7 +13421,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="7"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -14069,7 +14075,7 @@
         <v>0.159028</v>
       </c>
       <c r="BB3" s="25">
-        <f t="shared" ref="BB2:BB26" si="13">BA3/AL3*100</f>
+        <f t="shared" ref="BB3:BB26" si="13">BA3/AL3*100</f>
         <v>69.456066945606693</v>
       </c>
       <c r="BC3" s="22">
@@ -19044,7 +19050,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="7"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -19066,898 +19072,898 @@
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:20" ht="14.5">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="H1" s="36" t="s">
         <v>265</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="I1" s="36" t="s">
         <v>266</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="J1" s="36" t="s">
         <v>267</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="K1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="L1" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="M1" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="N1" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="O1" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="P1" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="Q1" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="R1" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="T1" s="36" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="34">
+        <v>1</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" s="34">
+        <v>-0.83103795646194334</v>
+      </c>
+      <c r="C3" s="34">
+        <v>1</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="B4" s="34">
+        <v>-0.64756766691649559</v>
+      </c>
+      <c r="C4" s="34">
+        <v>0.6012107405995275</v>
+      </c>
+      <c r="D4" s="34">
+        <v>1</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" s="34">
+        <v>-0.30628498679862604</v>
+      </c>
+      <c r="C5" s="34">
+        <v>0.31789162912995428</v>
+      </c>
+      <c r="D5" s="34">
+        <v>0.85445328915613739</v>
+      </c>
+      <c r="E5" s="34">
+        <v>1</v>
+      </c>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="34">
+        <v>-0.51656938083276649</v>
+      </c>
+      <c r="C6" s="34">
+        <v>0.50964499800004104</v>
+      </c>
+      <c r="D6" s="34">
+        <v>0.83819463973727582</v>
+      </c>
+      <c r="E6" s="34">
+        <v>0.88705605270552113</v>
+      </c>
+      <c r="F6" s="34">
+        <v>1</v>
+      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="34">
+        <v>-0.38855281756447019</v>
+      </c>
+      <c r="C7" s="34">
+        <v>0.37468916749537945</v>
+      </c>
+      <c r="D7" s="34">
+        <v>0.85320678284575402</v>
+      </c>
+      <c r="E7" s="34">
+        <v>0.96339520636912457</v>
+      </c>
+      <c r="F7" s="34">
+        <v>0.92016413231438643</v>
+      </c>
+      <c r="G7" s="34">
+        <v>1</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" s="34">
+        <v>-0.3347075599593155</v>
+      </c>
+      <c r="C8" s="34">
+        <v>0.17604954978801976</v>
+      </c>
+      <c r="D8" s="34">
+        <v>0.15501248981365984</v>
+      </c>
+      <c r="E8" s="34">
+        <v>-1.2819532382730033E-2</v>
+      </c>
+      <c r="F8" s="34">
+        <v>0.23110594923596042</v>
+      </c>
+      <c r="G8" s="34">
+        <v>0.23378803000983403</v>
+      </c>
+      <c r="H8" s="34">
+        <v>1</v>
+      </c>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="B9" s="34">
+        <v>-0.55115829380147052</v>
+      </c>
+      <c r="C9" s="34">
+        <v>0.44344796910101436</v>
+      </c>
+      <c r="D9" s="34">
+        <v>0.58455630452854634</v>
+      </c>
+      <c r="E9" s="34">
+        <v>0.52430373317432266</v>
+      </c>
+      <c r="F9" s="34">
+        <v>0.62504805265737584</v>
+      </c>
+      <c r="G9" s="34">
+        <v>0.53625224517503012</v>
+      </c>
+      <c r="H9" s="34">
+        <v>0.16041240197483436</v>
+      </c>
+      <c r="I9" s="34">
+        <v>1</v>
+      </c>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10" s="34">
+        <v>-0.394915743665462</v>
+      </c>
+      <c r="C10" s="34">
+        <v>0.39567209411992182</v>
+      </c>
+      <c r="D10" s="34">
+        <v>0.35487998903623541</v>
+      </c>
+      <c r="E10" s="34">
+        <v>0.34302303075749208</v>
+      </c>
+      <c r="F10" s="34">
+        <v>0.62905784865698744</v>
+      </c>
+      <c r="G10" s="34">
+        <v>0.36161231061063998</v>
+      </c>
+      <c r="H10" s="34">
+        <v>0.16064136263696124</v>
+      </c>
+      <c r="I10" s="34">
+        <v>0.3064495844024252</v>
+      </c>
+      <c r="J10" s="34">
+        <v>1</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" s="34">
+        <v>-0.56876222764696316</v>
+      </c>
+      <c r="C11" s="34">
+        <v>0.6451553119059521</v>
+      </c>
+      <c r="D11" s="34">
+        <v>0.86347444485845704</v>
+      </c>
+      <c r="E11" s="34">
+        <v>0.83496585280053659</v>
+      </c>
+      <c r="F11" s="34">
+        <v>0.84543225622478213</v>
+      </c>
+      <c r="G11" s="34">
+        <v>0.85664986736576187</v>
+      </c>
+      <c r="H11" s="34">
+        <v>0.12027609793303026</v>
+      </c>
+      <c r="I11" s="34">
+        <v>0.56558116422724947</v>
+      </c>
+      <c r="J11" s="34">
+        <v>0.32472136170499771</v>
+      </c>
+      <c r="K11" s="34">
+        <v>1</v>
+      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="34">
+        <v>-0.59063928710188673</v>
+      </c>
+      <c r="C12" s="34">
+        <v>0.63914342476203101</v>
+      </c>
+      <c r="D12" s="34">
+        <v>0.59226916941924301</v>
+      </c>
+      <c r="E12" s="34">
+        <v>0.54844627137633739</v>
+      </c>
+      <c r="F12" s="34">
+        <v>0.80559259727103627</v>
+      </c>
+      <c r="G12" s="34">
+        <v>0.58151651410529814</v>
+      </c>
+      <c r="H12" s="34">
+        <v>0.17025381586664404</v>
+      </c>
+      <c r="I12" s="34">
+        <v>0.44480703502664692</v>
+      </c>
+      <c r="J12" s="34">
+        <v>0.76166314418238179</v>
+      </c>
+      <c r="K12" s="34">
+        <v>0.68859237314150357</v>
+      </c>
+      <c r="L12" s="34">
+        <v>1</v>
+      </c>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" s="34">
+        <v>-0.48972871318514988</v>
+      </c>
+      <c r="C13" s="34">
+        <v>0.53558283296144704</v>
+      </c>
+      <c r="D13" s="34">
+        <v>0.7623729077426874</v>
+      </c>
+      <c r="E13" s="34">
+        <v>0.65237842065565044</v>
+      </c>
+      <c r="F13" s="34">
+        <v>0.55905094001758548</v>
+      </c>
+      <c r="G13" s="34">
+        <v>0.66766944985922516</v>
+      </c>
+      <c r="H13" s="34">
+        <v>0.11982442108488348</v>
+      </c>
+      <c r="I13" s="34">
+        <v>0.51878508002259682</v>
+      </c>
+      <c r="J13" s="34">
+        <v>8.2486152345413177E-3</v>
+      </c>
+      <c r="K13" s="34">
+        <v>0.7866569915777778</v>
+      </c>
+      <c r="L13" s="34">
+        <v>0.29340728041205044</v>
+      </c>
+      <c r="M13" s="34">
+        <v>1</v>
+      </c>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14" s="34">
+        <v>2.7199408798838948E-2</v>
+      </c>
+      <c r="C14" s="34">
+        <v>9.8622887335076223E-2</v>
+      </c>
+      <c r="D14" s="34">
+        <v>0.36868338096453462</v>
+      </c>
+      <c r="E14" s="34">
+        <v>0.44775951584050272</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0.20418130771702153</v>
+      </c>
+      <c r="G14" s="34">
+        <v>0.44442554335920803</v>
+      </c>
+      <c r="H14" s="34">
+        <v>-4.9960120499624859E-2</v>
+      </c>
+      <c r="I14" s="34">
+        <v>0.29977677303547517</v>
+      </c>
+      <c r="J14" s="34">
+        <v>-0.45183292548730364</v>
+      </c>
+      <c r="K14" s="34">
+        <v>0.50808929104806189</v>
+      </c>
+      <c r="L14" s="34">
+        <v>-0.10623133530108646</v>
+      </c>
+      <c r="M14" s="34">
+        <v>0.53125174468095548</v>
+      </c>
+      <c r="N14" s="34">
+        <v>1</v>
+      </c>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="34">
+        <v>-0.16016318613579136</v>
+      </c>
+      <c r="C15" s="34">
+        <v>4.5986950488812267E-2</v>
+      </c>
+      <c r="D15" s="34">
+        <v>0.12567494126511788</v>
+      </c>
+      <c r="E15" s="34">
+        <v>0.15960238265095331</v>
+      </c>
+      <c r="F15" s="34">
+        <v>0.37430566595057091</v>
+      </c>
+      <c r="G15" s="34">
+        <v>0.15574751180877472</v>
+      </c>
+      <c r="H15" s="34">
+        <v>9.9400127117200018E-2</v>
+      </c>
+      <c r="I15" s="34">
+        <v>6.9875532113250594E-2</v>
+      </c>
+      <c r="J15" s="34">
+        <v>0.67856791627885316</v>
+      </c>
+      <c r="K15" s="34">
+        <v>3.3230147220408789E-3</v>
+      </c>
+      <c r="L15" s="34">
+        <v>0.46949805375874459</v>
+      </c>
+      <c r="M15" s="34">
+        <v>-0.36529266819894424</v>
+      </c>
+      <c r="N15" s="34">
+        <v>-0.57226631255467519</v>
+      </c>
+      <c r="O15" s="34">
+        <v>1</v>
+      </c>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="34">
+        <v>-0.39769416198403817</v>
+      </c>
+      <c r="C16" s="34">
+        <v>0.11596924655597957</v>
+      </c>
+      <c r="D16" s="34">
+        <v>0.45797874838220642</v>
+      </c>
+      <c r="E16" s="34">
+        <v>0.30059434279799252</v>
+      </c>
+      <c r="F16" s="34">
+        <v>0.4175256562319129</v>
+      </c>
+      <c r="G16" s="34">
+        <v>0.31215300667399976</v>
+      </c>
+      <c r="H16" s="34">
+        <v>0.24613612598121343</v>
+      </c>
+      <c r="I16" s="34">
+        <v>0.44220977345059348</v>
+      </c>
+      <c r="J16" s="34">
+        <v>0.48246059493838162</v>
+      </c>
+      <c r="K16" s="34">
+        <v>0.22852925392301335</v>
+      </c>
+      <c r="L16" s="34">
+        <v>0.34373798401366229</v>
+      </c>
+      <c r="M16" s="34">
+        <v>7.3119096592524885E-2</v>
+      </c>
+      <c r="N16" s="34">
+        <v>-3.0475131915229041E-2</v>
+      </c>
+      <c r="O16" s="34">
+        <v>0.31377651363010323</v>
+      </c>
+      <c r="P16" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" s="34">
+        <v>-0.51029590509286904</v>
+      </c>
+      <c r="C17" s="34">
+        <v>0.42614851631274459</v>
+      </c>
+      <c r="D17" s="34">
+        <v>0.76992041013767454</v>
+      </c>
+      <c r="E17" s="34">
+        <v>0.72451202748709032</v>
+      </c>
+      <c r="F17" s="34">
+        <v>0.74077825591014668</v>
+      </c>
+      <c r="G17" s="34">
+        <v>0.74775074227668437</v>
+      </c>
+      <c r="H17" s="34">
+        <v>0.23355928445108232</v>
+      </c>
+      <c r="I17" s="34">
+        <v>0.41948199057232927</v>
+      </c>
+      <c r="J17" s="34">
+        <v>0.33808328338136784</v>
+      </c>
+      <c r="K17" s="34">
+        <v>0.63991671068607614</v>
+      </c>
+      <c r="L17" s="34">
+        <v>0.5637157383668937</v>
+      </c>
+      <c r="M17" s="34">
+        <v>0.47938337251557434</v>
+      </c>
+      <c r="N17" s="34">
+        <v>8.5960891028549091E-2</v>
+      </c>
+      <c r="O17" s="34">
+        <v>0.39553861642161253</v>
+      </c>
+      <c r="P17" s="34">
+        <v>0.23193920277837202</v>
+      </c>
+      <c r="Q17" s="34">
+        <v>1</v>
+      </c>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="B18" s="34">
+        <v>-0.57064213125570973</v>
+      </c>
+      <c r="C18" s="34">
+        <v>0.43932313415166391</v>
+      </c>
+      <c r="D18" s="34">
+        <v>0.8717149369108792</v>
+      </c>
+      <c r="E18" s="34">
+        <v>0.78570343662892872</v>
+      </c>
+      <c r="F18" s="34">
+        <v>0.70370409272693024</v>
+      </c>
+      <c r="G18" s="34">
+        <v>0.78683348512014095</v>
+      </c>
+      <c r="H18" s="34">
+        <v>0.13511210961095299</v>
+      </c>
+      <c r="I18" s="34">
+        <v>0.66525940371783476</v>
+      </c>
+      <c r="J18" s="34">
+        <v>0.20242296217748884</v>
+      </c>
+      <c r="K18" s="34">
+        <v>0.80124175307054735</v>
+      </c>
+      <c r="L18" s="34">
+        <v>0.39073409778880291</v>
+      </c>
+      <c r="M18" s="34">
+        <v>0.88392216844523008</v>
+      </c>
+      <c r="N18" s="34">
+        <v>0.43369100680623507</v>
+      </c>
+      <c r="O18" s="34">
+        <v>-8.3005053472864535E-2</v>
+      </c>
+      <c r="P18" s="34">
+        <v>0.36743124236475905</v>
+      </c>
+      <c r="Q18" s="34">
+        <v>0.65395071626310497</v>
+      </c>
+      <c r="R18" s="34">
+        <v>1</v>
+      </c>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="O1" s="37" t="s">
-        <v>262</v>
-      </c>
-      <c r="P1" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>276</v>
-      </c>
-      <c r="R1" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>278</v>
-      </c>
-      <c r="T1" s="37" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="35">
+      <c r="B19" s="34">
+        <v>-0.50059254518911589</v>
+      </c>
+      <c r="C19" s="34">
+        <v>0.46344956448372265</v>
+      </c>
+      <c r="D19" s="34">
+        <v>0.80544933392398455</v>
+      </c>
+      <c r="E19" s="34">
+        <v>0.75388231053896559</v>
+      </c>
+      <c r="F19" s="34">
+        <v>0.75042406743722867</v>
+      </c>
+      <c r="G19" s="34">
+        <v>0.76560972955471662</v>
+      </c>
+      <c r="H19" s="34">
+        <v>0.15963511718104392</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0.35536387473461201</v>
+      </c>
+      <c r="J19" s="34">
+        <v>0.36987264414732324</v>
+      </c>
+      <c r="K19" s="34">
+        <v>0.71643153971325169</v>
+      </c>
+      <c r="L19" s="34">
+        <v>0.57175337164315143</v>
+      </c>
+      <c r="M19" s="34">
+        <v>0.61832357143138794</v>
+      </c>
+      <c r="N19" s="34">
+        <v>0.13627185505030309</v>
+      </c>
+      <c r="O19" s="34">
+        <v>0.32416867041529118</v>
+      </c>
+      <c r="P19" s="34">
+        <v>0.1611825416866636</v>
+      </c>
+      <c r="Q19" s="34">
+        <v>0.92014658367073332</v>
+      </c>
+      <c r="R19" s="34">
+        <v>0.71586253311667503</v>
+      </c>
+      <c r="S19" s="34">
         <v>1</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="35" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" s="35">
-        <v>-0.83103795646194334</v>
-      </c>
-      <c r="C3" s="35">
-        <v>1</v>
-      </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="B4" s="35">
-        <v>-0.64756766691649559</v>
-      </c>
-      <c r="C4" s="35">
-        <v>0.6012107405995275</v>
-      </c>
-      <c r="D4" s="35">
-        <v>1</v>
-      </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="35" t="s">
-        <v>266</v>
-      </c>
-      <c r="B5" s="35">
-        <v>-0.30628498679862604</v>
-      </c>
-      <c r="C5" s="35">
-        <v>0.31789162912995428</v>
-      </c>
-      <c r="D5" s="35">
-        <v>0.85445328915613739</v>
-      </c>
-      <c r="E5" s="35">
-        <v>1</v>
-      </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="35" t="s">
-        <v>267</v>
-      </c>
-      <c r="B6" s="35">
-        <v>-0.51656938083276649</v>
-      </c>
-      <c r="C6" s="35">
-        <v>0.50964499800004104</v>
-      </c>
-      <c r="D6" s="35">
-        <v>0.83819463973727582</v>
-      </c>
-      <c r="E6" s="35">
-        <v>0.88705605270552113</v>
-      </c>
-      <c r="F6" s="35">
-        <v>1</v>
-      </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="35" t="s">
-        <v>268</v>
-      </c>
-      <c r="B7" s="35">
-        <v>-0.38855281756447019</v>
-      </c>
-      <c r="C7" s="35">
-        <v>0.37468916749537945</v>
-      </c>
-      <c r="D7" s="35">
-        <v>0.85320678284575402</v>
-      </c>
-      <c r="E7" s="35">
-        <v>0.96339520636912457</v>
-      </c>
-      <c r="F7" s="35">
-        <v>0.92016413231438643</v>
-      </c>
-      <c r="G7" s="35">
-        <v>1</v>
-      </c>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="35" t="s">
-        <v>269</v>
-      </c>
-      <c r="B8" s="35">
-        <v>-0.3347075599593155</v>
-      </c>
-      <c r="C8" s="35">
-        <v>0.17604954978801976</v>
-      </c>
-      <c r="D8" s="35">
-        <v>0.15501248981365984</v>
-      </c>
-      <c r="E8" s="35">
-        <v>-1.2819532382730033E-2</v>
-      </c>
-      <c r="F8" s="35">
-        <v>0.23110594923596042</v>
-      </c>
-      <c r="G8" s="35">
-        <v>0.23378803000983403</v>
-      </c>
-      <c r="H8" s="35">
-        <v>1</v>
-      </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="35" t="s">
-        <v>270</v>
-      </c>
-      <c r="B9" s="35">
-        <v>-0.55115829380147052</v>
-      </c>
-      <c r="C9" s="35">
-        <v>0.44344796910101436</v>
-      </c>
-      <c r="D9" s="35">
-        <v>0.58455630452854634</v>
-      </c>
-      <c r="E9" s="35">
-        <v>0.52430373317432266</v>
-      </c>
-      <c r="F9" s="35">
-        <v>0.62504805265737584</v>
-      </c>
-      <c r="G9" s="35">
-        <v>0.53625224517503012</v>
-      </c>
-      <c r="H9" s="35">
-        <v>0.16041240197483436</v>
-      </c>
-      <c r="I9" s="35">
-        <v>1</v>
-      </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="35" t="s">
-        <v>271</v>
-      </c>
-      <c r="B10" s="35">
-        <v>-0.394915743665462</v>
-      </c>
-      <c r="C10" s="35">
-        <v>0.39567209411992182</v>
-      </c>
-      <c r="D10" s="35">
-        <v>0.35487998903623541</v>
-      </c>
-      <c r="E10" s="35">
-        <v>0.34302303075749208</v>
-      </c>
-      <c r="F10" s="35">
-        <v>0.62905784865698744</v>
-      </c>
-      <c r="G10" s="35">
-        <v>0.36161231061063998</v>
-      </c>
-      <c r="H10" s="35">
-        <v>0.16064136263696124</v>
-      </c>
-      <c r="I10" s="35">
-        <v>0.3064495844024252</v>
-      </c>
-      <c r="J10" s="35">
-        <v>1</v>
-      </c>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="35" t="s">
-        <v>272</v>
-      </c>
-      <c r="B11" s="35">
-        <v>-0.56876222764696316</v>
-      </c>
-      <c r="C11" s="35">
-        <v>0.6451553119059521</v>
-      </c>
-      <c r="D11" s="35">
-        <v>0.86347444485845704</v>
-      </c>
-      <c r="E11" s="35">
-        <v>0.83496585280053659</v>
-      </c>
-      <c r="F11" s="35">
-        <v>0.84543225622478213</v>
-      </c>
-      <c r="G11" s="35">
-        <v>0.85664986736576187</v>
-      </c>
-      <c r="H11" s="35">
-        <v>0.12027609793303026</v>
-      </c>
-      <c r="I11" s="35">
-        <v>0.56558116422724947</v>
-      </c>
-      <c r="J11" s="35">
-        <v>0.32472136170499771</v>
-      </c>
-      <c r="K11" s="35">
-        <v>1</v>
-      </c>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="B12" s="35">
-        <v>-0.59063928710188673</v>
-      </c>
-      <c r="C12" s="35">
-        <v>0.63914342476203101</v>
-      </c>
-      <c r="D12" s="35">
-        <v>0.59226916941924301</v>
-      </c>
-      <c r="E12" s="35">
-        <v>0.54844627137633739</v>
-      </c>
-      <c r="F12" s="35">
-        <v>0.80559259727103627</v>
-      </c>
-      <c r="G12" s="35">
-        <v>0.58151651410529814</v>
-      </c>
-      <c r="H12" s="35">
-        <v>0.17025381586664404</v>
-      </c>
-      <c r="I12" s="35">
-        <v>0.44480703502664692</v>
-      </c>
-      <c r="J12" s="35">
-        <v>0.76166314418238179</v>
-      </c>
-      <c r="K12" s="35">
-        <v>0.68859237314150357</v>
-      </c>
-      <c r="L12" s="35">
-        <v>1</v>
-      </c>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="35" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" s="35">
-        <v>-0.48972871318514988</v>
-      </c>
-      <c r="C13" s="35">
-        <v>0.53558283296144704</v>
-      </c>
-      <c r="D13" s="35">
-        <v>0.7623729077426874</v>
-      </c>
-      <c r="E13" s="35">
-        <v>0.65237842065565044</v>
-      </c>
-      <c r="F13" s="35">
-        <v>0.55905094001758548</v>
-      </c>
-      <c r="G13" s="35">
-        <v>0.66766944985922516</v>
-      </c>
-      <c r="H13" s="35">
-        <v>0.11982442108488348</v>
-      </c>
-      <c r="I13" s="35">
-        <v>0.51878508002259682</v>
-      </c>
-      <c r="J13" s="35">
-        <v>8.2486152345413177E-3</v>
-      </c>
-      <c r="K13" s="35">
-        <v>0.7866569915777778</v>
-      </c>
-      <c r="L13" s="35">
-        <v>0.29340728041205044</v>
-      </c>
-      <c r="M13" s="35">
-        <v>1</v>
-      </c>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="35" t="s">
-        <v>274</v>
-      </c>
-      <c r="B14" s="35">
-        <v>2.7199408798838948E-2</v>
-      </c>
-      <c r="C14" s="35">
-        <v>9.8622887335076223E-2</v>
-      </c>
-      <c r="D14" s="35">
-        <v>0.36868338096453462</v>
-      </c>
-      <c r="E14" s="35">
-        <v>0.44775951584050272</v>
-      </c>
-      <c r="F14" s="35">
-        <v>0.20418130771702153</v>
-      </c>
-      <c r="G14" s="35">
-        <v>0.44442554335920803</v>
-      </c>
-      <c r="H14" s="35">
-        <v>-4.9960120499624859E-2</v>
-      </c>
-      <c r="I14" s="35">
-        <v>0.29977677303547517</v>
-      </c>
-      <c r="J14" s="35">
-        <v>-0.45183292548730364</v>
-      </c>
-      <c r="K14" s="35">
-        <v>0.50808929104806189</v>
-      </c>
-      <c r="L14" s="35">
-        <v>-0.10623133530108646</v>
-      </c>
-      <c r="M14" s="35">
-        <v>0.53125174468095548</v>
-      </c>
-      <c r="N14" s="35">
-        <v>1</v>
-      </c>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="35" t="s">
-        <v>262</v>
-      </c>
-      <c r="B15" s="35">
-        <v>-0.16016318613579136</v>
-      </c>
-      <c r="C15" s="35">
-        <v>4.5986950488812267E-2</v>
-      </c>
-      <c r="D15" s="35">
-        <v>0.12567494126511788</v>
-      </c>
-      <c r="E15" s="35">
-        <v>0.15960238265095331</v>
-      </c>
-      <c r="F15" s="35">
-        <v>0.37430566595057091</v>
-      </c>
-      <c r="G15" s="35">
-        <v>0.15574751180877472</v>
-      </c>
-      <c r="H15" s="35">
-        <v>9.9400127117200018E-2</v>
-      </c>
-      <c r="I15" s="35">
-        <v>6.9875532113250594E-2</v>
-      </c>
-      <c r="J15" s="35">
-        <v>0.67856791627885316</v>
-      </c>
-      <c r="K15" s="35">
-        <v>3.3230147220408789E-3</v>
-      </c>
-      <c r="L15" s="35">
-        <v>0.46949805375874459</v>
-      </c>
-      <c r="M15" s="35">
-        <v>-0.36529266819894424</v>
-      </c>
-      <c r="N15" s="35">
-        <v>-0.57226631255467519</v>
-      </c>
-      <c r="O15" s="35">
-        <v>1</v>
-      </c>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="35" t="s">
-        <v>275</v>
-      </c>
-      <c r="B16" s="35">
-        <v>-0.39769416198403817</v>
-      </c>
-      <c r="C16" s="35">
-        <v>0.11596924655597957</v>
-      </c>
-      <c r="D16" s="35">
-        <v>0.45797874838220642</v>
-      </c>
-      <c r="E16" s="35">
-        <v>0.30059434279799252</v>
-      </c>
-      <c r="F16" s="35">
-        <v>0.4175256562319129</v>
-      </c>
-      <c r="G16" s="35">
-        <v>0.31215300667399976</v>
-      </c>
-      <c r="H16" s="35">
-        <v>0.24613612598121343</v>
-      </c>
-      <c r="I16" s="35">
-        <v>0.44220977345059348</v>
-      </c>
-      <c r="J16" s="35">
-        <v>0.48246059493838162</v>
-      </c>
-      <c r="K16" s="35">
-        <v>0.22852925392301335</v>
-      </c>
-      <c r="L16" s="35">
-        <v>0.34373798401366229</v>
-      </c>
-      <c r="M16" s="35">
-        <v>7.3119096592524885E-2</v>
-      </c>
-      <c r="N16" s="35">
-        <v>-3.0475131915229041E-2</v>
-      </c>
-      <c r="O16" s="35">
-        <v>0.31377651363010323</v>
-      </c>
-      <c r="P16" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="B17" s="35">
-        <v>-0.51029590509286904</v>
-      </c>
-      <c r="C17" s="35">
-        <v>0.42614851631274459</v>
-      </c>
-      <c r="D17" s="35">
-        <v>0.76992041013767454</v>
-      </c>
-      <c r="E17" s="35">
-        <v>0.72451202748709032</v>
-      </c>
-      <c r="F17" s="35">
-        <v>0.74077825591014668</v>
-      </c>
-      <c r="G17" s="35">
-        <v>0.74775074227668437</v>
-      </c>
-      <c r="H17" s="35">
-        <v>0.23355928445108232</v>
-      </c>
-      <c r="I17" s="35">
-        <v>0.41948199057232927</v>
-      </c>
-      <c r="J17" s="35">
-        <v>0.33808328338136784</v>
-      </c>
-      <c r="K17" s="35">
-        <v>0.63991671068607614</v>
-      </c>
-      <c r="L17" s="35">
-        <v>0.5637157383668937</v>
-      </c>
-      <c r="M17" s="35">
-        <v>0.47938337251557434</v>
-      </c>
-      <c r="N17" s="35">
-        <v>8.5960891028549091E-2</v>
-      </c>
-      <c r="O17" s="35">
-        <v>0.39553861642161253</v>
-      </c>
-      <c r="P17" s="35">
-        <v>0.23193920277837202</v>
-      </c>
-      <c r="Q17" s="35">
-        <v>1</v>
-      </c>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="B18" s="35">
-        <v>-0.57064213125570973</v>
-      </c>
-      <c r="C18" s="35">
-        <v>0.43932313415166391</v>
-      </c>
-      <c r="D18" s="35">
-        <v>0.8717149369108792</v>
-      </c>
-      <c r="E18" s="35">
-        <v>0.78570343662892872</v>
-      </c>
-      <c r="F18" s="35">
-        <v>0.70370409272693024</v>
-      </c>
-      <c r="G18" s="35">
-        <v>0.78683348512014095</v>
-      </c>
-      <c r="H18" s="35">
-        <v>0.13511210961095299</v>
-      </c>
-      <c r="I18" s="35">
-        <v>0.66525940371783476</v>
-      </c>
-      <c r="J18" s="35">
-        <v>0.20242296217748884</v>
-      </c>
-      <c r="K18" s="35">
-        <v>0.80124175307054735</v>
-      </c>
-      <c r="L18" s="35">
-        <v>0.39073409778880291</v>
-      </c>
-      <c r="M18" s="35">
-        <v>0.88392216844523008</v>
-      </c>
-      <c r="N18" s="35">
-        <v>0.43369100680623507</v>
-      </c>
-      <c r="O18" s="35">
-        <v>-8.3005053472864535E-2</v>
-      </c>
-      <c r="P18" s="35">
-        <v>0.36743124236475905</v>
-      </c>
-      <c r="Q18" s="35">
-        <v>0.65395071626310497</v>
-      </c>
-      <c r="R18" s="35">
-        <v>1</v>
-      </c>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="35" t="s">
-        <v>278</v>
-      </c>
-      <c r="B19" s="35">
-        <v>-0.50059254518911589</v>
-      </c>
-      <c r="C19" s="35">
-        <v>0.46344956448372265</v>
-      </c>
-      <c r="D19" s="35">
-        <v>0.80544933392398455</v>
-      </c>
-      <c r="E19" s="35">
-        <v>0.75388231053896559</v>
-      </c>
-      <c r="F19" s="35">
-        <v>0.75042406743722867</v>
-      </c>
-      <c r="G19" s="35">
-        <v>0.76560972955471662</v>
-      </c>
-      <c r="H19" s="35">
-        <v>0.15963511718104392</v>
-      </c>
-      <c r="I19" s="35">
-        <v>0.35536387473461201</v>
-      </c>
-      <c r="J19" s="35">
-        <v>0.36987264414732324</v>
-      </c>
-      <c r="K19" s="35">
-        <v>0.71643153971325169</v>
-      </c>
-      <c r="L19" s="35">
-        <v>0.57175337164315143</v>
-      </c>
-      <c r="M19" s="35">
-        <v>0.61832357143138794</v>
-      </c>
-      <c r="N19" s="35">
-        <v>0.13627185505030309</v>
-      </c>
-      <c r="O19" s="35">
-        <v>0.32416867041529118</v>
-      </c>
-      <c r="P19" s="35">
-        <v>0.1611825416866636</v>
-      </c>
-      <c r="Q19" s="35">
-        <v>0.92014658367073332</v>
-      </c>
-      <c r="R19" s="35">
-        <v>0.71586253311667503</v>
-      </c>
-      <c r="S19" s="35">
-        <v>1</v>
-      </c>
-      <c r="T19" s="35"/>
+      <c r="T19" s="34"/>
     </row>
     <row r="20" spans="1:20" ht="14.5" thickBot="1">
-      <c r="A20" s="36" t="s">
-        <v>263</v>
-      </c>
-      <c r="B20" s="36">
+      <c r="A20" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="B20" s="35">
         <v>-0.27087081961014442</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="35">
         <v>0.33309406130401947</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D20" s="35">
         <v>0.5267891112754628</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="35">
         <v>0.48615462283281191</v>
       </c>
-      <c r="F20" s="36">
+      <c r="F20" s="35">
         <v>0.44908227118683003</v>
       </c>
-      <c r="G20" s="36">
+      <c r="G20" s="35">
         <v>0.47243070033601403</v>
       </c>
-      <c r="H20" s="36">
+      <c r="H20" s="35">
         <v>-3.9599057555925514E-2</v>
       </c>
-      <c r="I20" s="36">
+      <c r="I20" s="35">
         <v>9.0498771333422254E-2</v>
       </c>
-      <c r="J20" s="36">
+      <c r="J20" s="35">
         <v>0.26943034276034844</v>
       </c>
-      <c r="K20" s="36">
+      <c r="K20" s="35">
         <v>0.54844995657459128</v>
       </c>
-      <c r="L20" s="36">
+      <c r="L20" s="35">
         <v>0.34338336311335516</v>
       </c>
-      <c r="M20" s="36">
+      <c r="M20" s="35">
         <v>0.60301086282593641</v>
       </c>
-      <c r="N20" s="36">
+      <c r="N20" s="35">
         <v>0.16791772960187273</v>
       </c>
-      <c r="O20" s="36">
+      <c r="O20" s="35">
         <v>5.9645475525651033E-2</v>
       </c>
-      <c r="P20" s="36">
+      <c r="P20" s="35">
         <v>-3.3074682481904372E-2</v>
       </c>
-      <c r="Q20" s="36">
+      <c r="Q20" s="35">
         <v>0.3875875381604294</v>
       </c>
-      <c r="R20" s="36">
+      <c r="R20" s="35">
         <v>0.52214958870206141</v>
       </c>
-      <c r="S20" s="36">
+      <c r="S20" s="35">
         <v>0.71760322506563579</v>
       </c>
-      <c r="T20" s="36">
+      <c r="T20" s="35">
         <v>1</v>
       </c>
     </row>
@@ -19976,7 +19982,7 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="14.5"/>
@@ -20005,68 +20011,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="53" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>244</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>246</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="L1" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="J1" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="K1" s="31" t="s">
+      <c r="M1" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="S1" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="T1" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="U1" s="33" t="s">
         <v>259</v>
-      </c>
-      <c r="L1" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="N1" s="38" t="s">
-        <v>273</v>
-      </c>
-      <c r="O1" s="34" t="s">
-        <v>251</v>
-      </c>
-      <c r="P1" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q1" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="R1" s="34" t="s">
-        <v>254</v>
-      </c>
-      <c r="S1" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="T1" s="34" t="s">
-        <v>256</v>
-      </c>
-      <c r="U1" s="34" t="s">
-        <v>263</v>
       </c>
       <c r="V1" s="18"/>
     </row>
@@ -20077,13 +20083,13 @@
       <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="31">
         <v>292</v>
       </c>
       <c r="D2" s="28">
         <v>20</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="32">
         <v>2.3449999999999998</v>
       </c>
       <c r="F2" s="28">
@@ -20095,7 +20101,7 @@
       <c r="H2" s="28">
         <v>13.6</v>
       </c>
-      <c r="I2" s="33">
+      <c r="I2" s="32">
         <v>1.182608695652174</v>
       </c>
       <c r="J2" s="28">
@@ -20125,7 +20131,7 @@
       <c r="R2" s="28">
         <v>4</v>
       </c>
-      <c r="S2" s="33">
+      <c r="S2" s="32">
         <v>2.0149999999999997</v>
       </c>
       <c r="T2" s="28">
@@ -20143,13 +20149,13 @@
       <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="31">
         <v>292</v>
       </c>
       <c r="D3" s="28">
         <v>26</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="32">
         <v>1.9700000000000002</v>
       </c>
       <c r="F3" s="28">
@@ -20161,7 +20167,7 @@
       <c r="H3" s="28">
         <v>15.2</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="32">
         <v>1.1874999999999998</v>
       </c>
       <c r="J3" s="28">
@@ -20191,7 +20197,7 @@
       <c r="R3" s="28">
         <v>5</v>
       </c>
-      <c r="S3" s="33">
+      <c r="S3" s="32">
         <v>1.7250000000000001</v>
       </c>
       <c r="T3" s="28">
@@ -20209,13 +20215,13 @@
       <c r="B4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>292</v>
       </c>
       <c r="D4" s="28">
         <v>10</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="32">
         <v>2.0149999999999997</v>
       </c>
       <c r="F4" s="28">
@@ -20227,7 +20233,7 @@
       <c r="H4" s="28">
         <v>14.4</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="32">
         <v>1.2100840336134453</v>
       </c>
       <c r="J4" s="28">
@@ -20257,7 +20263,7 @@
       <c r="R4" s="28">
         <v>7</v>
       </c>
-      <c r="S4" s="33">
+      <c r="S4" s="32">
         <v>2.125</v>
       </c>
       <c r="T4" s="28">
@@ -20275,13 +20281,13 @@
       <c r="B5" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>292</v>
       </c>
       <c r="D5" s="28">
         <v>20</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <v>2.2649999999999997</v>
       </c>
       <c r="F5" s="28">
@@ -20293,7 +20299,7 @@
       <c r="H5" s="28">
         <v>13</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="32">
         <v>1.0833333333333333</v>
       </c>
       <c r="J5" s="28">
@@ -20323,7 +20329,7 @@
       <c r="R5" s="28">
         <v>3</v>
       </c>
-      <c r="S5" s="33">
+      <c r="S5" s="32">
         <v>1.52</v>
       </c>
       <c r="T5" s="28">
@@ -20341,13 +20347,13 @@
       <c r="B6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>292</v>
       </c>
       <c r="D6" s="28">
         <v>18</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="32">
         <v>1.885</v>
       </c>
       <c r="F6" s="28">
@@ -20359,7 +20365,7 @@
       <c r="H6" s="28">
         <v>9.5</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="32">
         <v>1.1176470588235294</v>
       </c>
       <c r="J6" s="28">
@@ -20389,7 +20395,7 @@
       <c r="R6" s="28">
         <v>2</v>
       </c>
-      <c r="S6" s="33">
+      <c r="S6" s="32">
         <v>1.3199999999999998</v>
       </c>
       <c r="T6" s="28">
@@ -20407,13 +20413,13 @@
       <c r="B7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>292</v>
       </c>
       <c r="D7" s="28">
         <v>18</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>3.585</v>
       </c>
       <c r="F7" s="28">
@@ -20425,7 +20431,7 @@
       <c r="H7" s="28">
         <v>27.5</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="32">
         <v>1.0576923076923077</v>
       </c>
       <c r="J7" s="28">
@@ -20455,7 +20461,7 @@
       <c r="R7" s="28">
         <v>10</v>
       </c>
-      <c r="S7" s="33">
+      <c r="S7" s="32">
         <v>3.02</v>
       </c>
       <c r="T7" s="28">
@@ -20473,13 +20479,13 @@
       <c r="B8" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>292</v>
       </c>
       <c r="D8" s="28">
         <v>18</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <v>3.4550000000000001</v>
       </c>
       <c r="F8" s="28">
@@ -20491,7 +20497,7 @@
       <c r="H8" s="28">
         <v>30</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="32">
         <v>1.5384615384615385</v>
       </c>
       <c r="J8" s="28">
@@ -20521,7 +20527,7 @@
       <c r="R8" s="28">
         <v>6</v>
       </c>
-      <c r="S8" s="33">
+      <c r="S8" s="32">
         <v>2.0549999999999997</v>
       </c>
       <c r="T8" s="28">
@@ -20539,13 +20545,13 @@
       <c r="B9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>292</v>
       </c>
       <c r="D9" s="28">
         <v>16</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <v>3.88</v>
       </c>
       <c r="F9" s="28">
@@ -20557,7 +20563,7 @@
       <c r="H9" s="28">
         <v>27.7</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="32">
         <v>1.398989898989899</v>
       </c>
       <c r="J9" s="28">
@@ -20587,7 +20593,7 @@
       <c r="R9" s="28">
         <v>8</v>
       </c>
-      <c r="S9" s="33">
+      <c r="S9" s="32">
         <v>2.6399999999999997</v>
       </c>
       <c r="T9" s="28">
@@ -20605,13 +20611,13 @@
       <c r="B10" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>292</v>
       </c>
       <c r="D10" s="28">
         <v>16</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <v>3.645</v>
       </c>
       <c r="F10" s="28">
@@ -20623,7 +20629,7 @@
       <c r="H10" s="28">
         <v>35.799999999999997</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="32">
         <v>1.1973244147157189</v>
       </c>
       <c r="J10" s="28">
@@ -20653,7 +20659,7 @@
       <c r="R10" s="28">
         <v>8</v>
       </c>
-      <c r="S10" s="33">
+      <c r="S10" s="32">
         <v>2.9649999999999999</v>
       </c>
       <c r="T10" s="28">
@@ -20671,13 +20677,13 @@
       <c r="B11" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <v>292</v>
       </c>
       <c r="D11" s="28">
         <v>18</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="32">
         <v>3.4050000000000002</v>
       </c>
       <c r="F11" s="28">
@@ -20689,7 +20695,7 @@
       <c r="H11" s="28">
         <v>29.7</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="32">
         <v>1.0999999999999999</v>
       </c>
       <c r="J11" s="28">
@@ -20719,7 +20725,7 @@
       <c r="R11" s="28">
         <v>8</v>
       </c>
-      <c r="S11" s="33">
+      <c r="S11" s="32">
         <v>2.9550000000000001</v>
       </c>
       <c r="T11" s="28">
@@ -20737,13 +20743,13 @@
       <c r="B12" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>292</v>
       </c>
       <c r="D12" s="28">
         <v>14</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="32">
         <v>5.2650000000000006</v>
       </c>
       <c r="F12" s="28">
@@ -20755,7 +20761,7 @@
       <c r="H12" s="28">
         <v>55</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="32">
         <v>1.1702127659574468</v>
       </c>
       <c r="J12" s="28">
@@ -20785,7 +20791,7 @@
       <c r="R12" s="28">
         <v>9</v>
       </c>
-      <c r="S12" s="33">
+      <c r="S12" s="32">
         <v>5.01</v>
       </c>
       <c r="T12" s="28">
@@ -20803,13 +20809,13 @@
       <c r="B13" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="31">
         <v>292</v>
       </c>
       <c r="D13" s="28">
         <v>16</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <v>5.4</v>
       </c>
       <c r="F13" s="28">
@@ -20821,7 +20827,7 @@
       <c r="H13" s="28">
         <v>54</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="32">
         <v>1.0588235294117647</v>
       </c>
       <c r="J13" s="28">
@@ -20851,7 +20857,7 @@
       <c r="R13" s="28">
         <v>14</v>
       </c>
-      <c r="S13" s="33">
+      <c r="S13" s="32">
         <v>4.2799999999999994</v>
       </c>
       <c r="T13" s="28">
@@ -20869,13 +20875,13 @@
       <c r="B14" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="31">
         <v>292</v>
       </c>
       <c r="D14" s="28">
         <v>12</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="32">
         <v>4.9450000000000003</v>
       </c>
       <c r="F14" s="28">
@@ -20887,7 +20893,7 @@
       <c r="H14" s="28">
         <v>51</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="32">
         <v>1.5454545454545454</v>
       </c>
       <c r="J14" s="28">
@@ -20917,7 +20923,7 @@
       <c r="R14" s="28">
         <v>10</v>
       </c>
-      <c r="S14" s="33">
+      <c r="S14" s="32">
         <v>4.0049999999999999</v>
       </c>
       <c r="T14" s="28">
@@ -20935,13 +20941,13 @@
       <c r="B15" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>292</v>
       </c>
       <c r="D15" s="28">
         <v>18</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="32">
         <v>6.35</v>
       </c>
       <c r="F15" s="28">
@@ -20953,7 +20959,7 @@
       <c r="H15" s="28">
         <v>73</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="32">
         <v>1.2586206896551724</v>
       </c>
       <c r="J15" s="28">
@@ -20983,7 +20989,7 @@
       <c r="R15" s="28">
         <v>9</v>
       </c>
-      <c r="S15" s="33">
+      <c r="S15" s="32">
         <v>6.6349999999999998</v>
       </c>
       <c r="T15" s="28">
@@ -21001,13 +21007,13 @@
       <c r="B16" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <v>292</v>
       </c>
       <c r="D16" s="28">
         <v>20</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="32">
         <v>5.61</v>
       </c>
       <c r="F16" s="28">
@@ -21019,7 +21025,7 @@
       <c r="H16" s="28">
         <v>43</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="32">
         <v>1.0487804878048781</v>
       </c>
       <c r="J16" s="28">
@@ -21049,7 +21055,7 @@
       <c r="R16" s="28">
         <v>8</v>
       </c>
-      <c r="S16" s="33">
+      <c r="S16" s="32">
         <v>2.98</v>
       </c>
       <c r="T16" s="28">
@@ -21067,13 +21073,13 @@
       <c r="B17" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="31">
         <v>52</v>
       </c>
       <c r="D17" s="28">
         <v>27</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <v>4.6050000000000004</v>
       </c>
       <c r="F17" s="28">
@@ -21085,7 +21091,7 @@
       <c r="H17" s="28">
         <v>33.5</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="32">
         <v>1.1964285714285714</v>
       </c>
       <c r="J17" s="28">
@@ -21115,7 +21121,7 @@
       <c r="R17" s="28">
         <v>6</v>
       </c>
-      <c r="S17" s="33">
+      <c r="S17" s="32">
         <v>5.2650000000000006</v>
       </c>
       <c r="T17" s="28">
@@ -21133,13 +21139,13 @@
       <c r="B18" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <v>52</v>
       </c>
       <c r="D18" s="28">
         <v>26</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="32">
         <v>5.0600000000000005</v>
       </c>
       <c r="F18" s="28">
@@ -21151,7 +21157,7 @@
       <c r="H18" s="28">
         <v>31</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="32">
         <v>1.3478260869565217</v>
       </c>
       <c r="J18" s="28">
@@ -21181,7 +21187,7 @@
       <c r="R18" s="28">
         <v>7</v>
       </c>
-      <c r="S18" s="33">
+      <c r="S18" s="32">
         <v>3.6850000000000001</v>
       </c>
       <c r="T18" s="28">
@@ -21199,13 +21205,13 @@
       <c r="B19" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>52</v>
       </c>
       <c r="D19" s="28">
         <v>34</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="32">
         <v>6.5950000000000006</v>
       </c>
       <c r="F19" s="28">
@@ -21217,7 +21223,7 @@
       <c r="H19" s="28">
         <v>50</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="32">
         <v>1.3157894736842106</v>
       </c>
       <c r="J19" s="28">
@@ -21247,7 +21253,7 @@
       <c r="R19" s="28">
         <v>17</v>
       </c>
-      <c r="S19" s="33">
+      <c r="S19" s="32">
         <v>4.7699999999999996</v>
       </c>
       <c r="T19" s="28">
@@ -21265,13 +21271,13 @@
       <c r="B20" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>52</v>
       </c>
       <c r="D20" s="28">
         <v>33</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <v>6.51</v>
       </c>
       <c r="F20" s="28">
@@ -21283,7 +21289,7 @@
       <c r="H20" s="28">
         <v>75.5</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="32">
         <v>1.4245283018867925</v>
       </c>
       <c r="J20" s="28">
@@ -21313,7 +21319,7 @@
       <c r="R20" s="28">
         <v>14</v>
       </c>
-      <c r="S20" s="33">
+      <c r="S20" s="32">
         <v>5.7200000000000006</v>
       </c>
       <c r="T20" s="28">
@@ -21331,13 +21337,13 @@
       <c r="B21" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <v>52</v>
       </c>
       <c r="D21" s="28">
         <v>27</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="32">
         <v>4.5549999999999997</v>
       </c>
       <c r="F21" s="28">
@@ -21349,7 +21355,7 @@
       <c r="H21" s="28">
         <v>28</v>
       </c>
-      <c r="I21" s="33">
+      <c r="I21" s="32">
         <v>1.5555555555555556</v>
       </c>
       <c r="J21" s="28">
@@ -21379,7 +21385,7 @@
       <c r="R21" s="28">
         <v>11</v>
       </c>
-      <c r="S21" s="33">
+      <c r="S21" s="32">
         <v>4.4250000000000007</v>
       </c>
       <c r="T21" s="28">
@@ -21392,18 +21398,18 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="29" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <v>75</v>
       </c>
       <c r="D22" s="28">
         <v>45</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <v>7.335</v>
       </c>
       <c r="F22" s="28">
@@ -21415,7 +21421,7 @@
       <c r="H22" s="28">
         <v>49</v>
       </c>
-      <c r="I22" s="33">
+      <c r="I22" s="32">
         <v>1.2564102564102564</v>
       </c>
       <c r="J22" s="28">
@@ -21445,7 +21451,7 @@
       <c r="R22" s="28">
         <v>11</v>
       </c>
-      <c r="S22" s="33">
+      <c r="S22" s="32">
         <v>6.7949999999999999</v>
       </c>
       <c r="T22" s="28">
@@ -21458,18 +21464,18 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="29" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="31">
         <v>75</v>
       </c>
       <c r="D23" s="28">
         <v>40</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="32">
         <v>6.6150000000000002</v>
       </c>
       <c r="F23" s="28">
@@ -21481,7 +21487,7 @@
       <c r="H23" s="28">
         <v>43</v>
       </c>
-      <c r="I23" s="33">
+      <c r="I23" s="32">
         <v>1.1621621621621621</v>
       </c>
       <c r="J23" s="28">
@@ -21511,7 +21517,7 @@
       <c r="R23" s="28">
         <v>11</v>
       </c>
-      <c r="S23" s="33">
+      <c r="S23" s="32">
         <v>4.6550000000000002</v>
       </c>
       <c r="T23" s="28">
@@ -21524,18 +21530,18 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="29" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <v>75</v>
       </c>
       <c r="D24" s="28">
         <v>39</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="32">
         <v>6.13</v>
       </c>
       <c r="F24" s="28">
@@ -21547,7 +21553,7 @@
       <c r="H24" s="28">
         <v>62</v>
       </c>
-      <c r="I24" s="33">
+      <c r="I24" s="32">
         <v>1.3478260869565217</v>
       </c>
       <c r="J24" s="28">
@@ -21577,7 +21583,7 @@
       <c r="R24" s="28">
         <v>12</v>
       </c>
-      <c r="S24" s="33">
+      <c r="S24" s="32">
         <v>3.5049999999999999</v>
       </c>
       <c r="T24" s="28">
@@ -21590,18 +21596,18 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="29" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>75</v>
       </c>
       <c r="D25" s="28">
         <v>30</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="32">
         <v>7.8150000000000004</v>
       </c>
       <c r="F25" s="28">
@@ -21613,7 +21619,7 @@
       <c r="H25" s="28">
         <v>51</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="32">
         <v>1.1086956521739131</v>
       </c>
       <c r="J25" s="28">
@@ -21643,7 +21649,7 @@
       <c r="R25" s="28">
         <v>11</v>
       </c>
-      <c r="S25" s="33">
+      <c r="S25" s="32">
         <v>5.95</v>
       </c>
       <c r="T25" s="28">
@@ -21656,18 +21662,18 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="29" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="31">
         <v>75</v>
       </c>
       <c r="D26" s="28">
         <v>44</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="32">
         <v>5.5600000000000005</v>
       </c>
       <c r="F26" s="28">
@@ -21679,7 +21685,7 @@
       <c r="H26" s="28">
         <v>53</v>
       </c>
-      <c r="I26" s="33">
+      <c r="I26" s="32">
         <v>1.3947368421052631</v>
       </c>
       <c r="J26" s="28">
@@ -21709,7 +21715,7 @@
       <c r="R26" s="28">
         <v>10</v>
       </c>
-      <c r="S26" s="33">
+      <c r="S26" s="32">
         <v>3.54</v>
       </c>
       <c r="T26" s="28">
@@ -21721,7 +21727,7 @@
       <c r="V26" s="16"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21751,11 +21757,11 @@
         <v>44704</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6"/>
+  <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>